<commit_message>
add in some stats - method to obtain
</commit_message>
<xml_diff>
--- a/scint_fp/path_LOGS/DOY_in_LOG_IMU_BTT.xlsx
+++ b/scint_fp/path_LOGS/DOY_in_LOG_IMU_BTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\scintillometer_footprints\scint_fp\path_LOGS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E2C5B-823C-4A5A-8570-34A832BA92D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5056FB21-5625-4B23-A037-90C9BCCD03D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,12 +378,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,11 +542,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -911,7 +904,7 @@
   <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,28 +991,28 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B4" s="2">
         <v>197</v>
       </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1050,28 +1043,28 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="2">
         <v>195</v>
       </c>
-      <c r="C6" s="3">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="C6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1258,28 +1251,28 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="A14" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B14" s="2">
         <v>187</v>
       </c>
-      <c r="C14" s="3">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1882,28 +1875,28 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B38" s="3">
+      <c r="A38" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B38" s="2">
         <v>135</v>
       </c>
-      <c r="C38" s="3">
-        <v>10</v>
-      </c>
-      <c r="D38" s="3">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" s="3" t="s">
+      <c r="C38" s="2">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>